<commit_message>
save + read methods added to lpinstance
</commit_message>
<xml_diff>
--- a/Rapport/miplib2010_complete_gurobi.xlsx
+++ b/Rapport/miplib2010_complete_gurobi.xlsx
@@ -17,7 +17,7 @@
     <definedName name="MIPLIB_test" localSheetId="2">Blad2!$A$1:$B$362</definedName>
     <definedName name="MIPLIB_test" localSheetId="1">miplibobjectives!$G$1:$H$362</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -2266,7 +2266,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="174" formatCode="#,##0.00000000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00000000"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -2769,11 +2769,11 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="174" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="174" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -2820,31 +2820,7 @@
     <cellStyle name="Verklarende tekst" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Waarschuwingstekst" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC4D79B"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC4D79B"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC4D79B"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -6079,8 +6055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E365"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A418" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6119,7 +6095,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="8">
-        <f>C2-B2</f>
+        <f t="shared" ref="E2:E65" si="0">C2-B2</f>
         <v>0</v>
       </c>
     </row>
@@ -6137,7 +6113,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="8">
-        <f>C3-B3</f>
+        <f t="shared" si="0"/>
         <v>1.4632996681029908E-7</v>
       </c>
     </row>
@@ -6155,7 +6131,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="8">
-        <f>C4-B4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6173,7 +6149,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="8">
-        <f>C5-B5</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6191,7 +6167,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="8">
-        <f>C6-B6</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6209,7 +6185,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="8">
-        <f>C7-B7</f>
+        <f t="shared" si="0"/>
         <v>-2.6829260235672336E-7</v>
       </c>
     </row>
@@ -6227,7 +6203,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="8">
-        <f>C8-B8</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6245,7 +6221,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="8">
-        <f>C9-B9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6263,7 +6239,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="8">
-        <f>C10-B10</f>
+        <f t="shared" si="0"/>
         <v>-4.2348005990788806E-8</v>
       </c>
     </row>
@@ -6281,7 +6257,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="8">
-        <f>C11-B11</f>
+        <f t="shared" si="0"/>
         <v>-1.4285710037142962E-7</v>
       </c>
     </row>
@@ -6299,7 +6275,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="8">
-        <f>C12-B12</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6317,7 +6293,7 @@
         <v>11</v>
       </c>
       <c r="E13" s="8">
-        <f>C13-B13</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6335,7 +6311,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="8">
-        <f>C14-B14</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6353,7 +6329,7 @@
         <v>11</v>
       </c>
       <c r="E15" s="8">
-        <f>C15-B15</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6371,7 +6347,7 @@
         <v>11</v>
       </c>
       <c r="E16" s="8">
-        <f>C16-B16</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6389,7 +6365,7 @@
         <v>16</v>
       </c>
       <c r="E17" s="8">
-        <f>C17-B17</f>
+        <f t="shared" si="0"/>
         <v>-4.4836014012616943E-8</v>
       </c>
     </row>
@@ -6407,7 +6383,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="8">
-        <f>C18-B18</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6425,7 +6401,7 @@
         <v>16</v>
       </c>
       <c r="E19" s="8">
-        <f>C19-B19</f>
+        <f t="shared" si="0"/>
         <v>-3.6937035474693403E-7</v>
       </c>
     </row>
@@ -6443,7 +6419,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="8">
-        <f>C20-B20</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6461,7 +6437,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="8">
-        <f>C21-B21</f>
+        <f t="shared" si="0"/>
         <v>-4.3896640988805302E-7</v>
       </c>
     </row>
@@ -6479,7 +6455,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="8">
-        <f>C22-B22</f>
+        <f t="shared" si="0"/>
         <v>-3.8743019104003906E-7</v>
       </c>
     </row>
@@ -6497,7 +6473,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="8">
-        <f>C23-B23</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6515,7 +6491,7 @@
         <v>0</v>
       </c>
       <c r="E24" s="8">
-        <f>C24-B24</f>
+        <f t="shared" si="0"/>
         <v>3.3333339999330747E-7</v>
       </c>
     </row>
@@ -6533,7 +6509,7 @@
         <v>0</v>
       </c>
       <c r="E25" s="8">
-        <f>C25-B25</f>
+        <f t="shared" si="0"/>
         <v>1.2245689973156004E-7</v>
       </c>
     </row>
@@ -6551,7 +6527,7 @@
         <v>0</v>
       </c>
       <c r="E26" s="8">
-        <f>C26-B26</f>
+        <f t="shared" si="0"/>
         <v>-3.8911279887088313E-7</v>
       </c>
     </row>
@@ -6569,7 +6545,7 @@
         <v>0</v>
       </c>
       <c r="E27" s="8">
-        <f>C27-B27</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6587,7 +6563,7 @@
         <v>0</v>
       </c>
       <c r="E28" s="8">
-        <f>C28-B28</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6605,7 +6581,7 @@
         <v>16</v>
       </c>
       <c r="E29" s="8">
-        <f>C29-B29</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6623,7 +6599,7 @@
         <v>0</v>
       </c>
       <c r="E30" s="8">
-        <f>C30-B30</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6641,7 +6617,7 @@
         <v>0</v>
       </c>
       <c r="E31" s="8">
-        <f>C31-B31</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6659,7 +6635,7 @@
         <v>0</v>
       </c>
       <c r="E32" s="8">
-        <f>C32-B32</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6677,7 +6653,7 @@
         <v>0</v>
       </c>
       <c r="E33" s="8">
-        <f>C33-B33</f>
+        <f t="shared" si="0"/>
         <v>3.7735901514679426E-7</v>
       </c>
     </row>
@@ -6695,7 +6671,7 @@
         <v>0</v>
       </c>
       <c r="E34" s="8">
-        <f>C34-B34</f>
+        <f t="shared" si="0"/>
         <v>3.529394234647043E-7</v>
       </c>
     </row>
@@ -6713,7 +6689,7 @@
         <v>0</v>
       </c>
       <c r="E35" s="8">
-        <f>C35-B35</f>
+        <f t="shared" si="0"/>
         <v>5.882975528948009E-8</v>
       </c>
     </row>
@@ -6731,7 +6707,7 @@
         <v>0</v>
       </c>
       <c r="E36" s="8">
-        <f>C36-B36</f>
+        <f t="shared" si="0"/>
         <v>-3.529394234647043E-7</v>
       </c>
     </row>
@@ -6749,7 +6725,7 @@
         <v>0</v>
       </c>
       <c r="E37" s="8">
-        <f>C37-B37</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6767,7 +6743,7 @@
         <v>0</v>
       </c>
       <c r="E38" s="8">
-        <f>C38-B38</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6785,7 +6761,7 @@
         <v>0</v>
       </c>
       <c r="E39" s="8">
-        <f>C39-B39</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6803,7 +6779,7 @@
         <v>0</v>
       </c>
       <c r="E40" s="8">
-        <f>C40-B40</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6821,7 +6797,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="8">
-        <f>C41-B41</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6839,7 +6815,7 @@
         <v>16</v>
       </c>
       <c r="E42" s="8">
-        <f>C42-B42</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6857,7 +6833,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="8">
-        <f>C43-B43</f>
+        <f t="shared" si="0"/>
         <v>2.0899460650980473E-7</v>
       </c>
     </row>
@@ -6875,7 +6851,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="8">
-        <f>C44-B44</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6893,7 +6869,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="8">
-        <f>C45-B45</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6911,7 +6887,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="8">
-        <f>C46-B46</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6929,7 +6905,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="8">
-        <f>C47-B47</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6947,7 +6923,7 @@
         <v>0</v>
       </c>
       <c r="E48" s="8">
-        <f>C48-B48</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6965,7 +6941,7 @@
         <v>0</v>
       </c>
       <c r="E49" s="8">
-        <f>C49-B49</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -6983,7 +6959,7 @@
         <v>0</v>
       </c>
       <c r="E50" s="8">
-        <f>C50-B50</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7001,7 +6977,7 @@
         <v>0</v>
       </c>
       <c r="E51" s="8">
-        <f>C51-B51</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7019,7 +6995,7 @@
         <v>0</v>
       </c>
       <c r="E52" s="8">
-        <f>C52-B52</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7037,7 +7013,7 @@
         <v>11</v>
       </c>
       <c r="E53" s="8">
-        <f>C53-B53</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7055,7 +7031,7 @@
         <v>11</v>
       </c>
       <c r="E54" s="8">
-        <f>C54-B54</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7073,7 +7049,7 @@
         <v>11</v>
       </c>
       <c r="E55" s="8">
-        <f>C55-B55</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7091,7 +7067,7 @@
         <v>11</v>
       </c>
       <c r="E56" s="8">
-        <f>C56-B56</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7109,7 +7085,7 @@
         <v>0</v>
       </c>
       <c r="E57" s="8">
-        <f>C57-B57</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7127,7 +7103,7 @@
         <v>0</v>
       </c>
       <c r="E58" s="8">
-        <f>C58-B58</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7145,7 +7121,7 @@
         <v>0</v>
       </c>
       <c r="E59" s="8">
-        <f>C59-B59</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7163,7 +7139,7 @@
         <v>0</v>
       </c>
       <c r="E60" s="8">
-        <f>C60-B60</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7181,7 +7157,7 @@
         <v>11</v>
       </c>
       <c r="E61" s="8">
-        <f>C61-B61</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7199,7 +7175,7 @@
         <v>11</v>
       </c>
       <c r="E62" s="8">
-        <f>C62-B62</f>
+        <f t="shared" si="0"/>
         <v>1.0004441719502211E-11</v>
       </c>
     </row>
@@ -7217,7 +7193,7 @@
         <v>0</v>
       </c>
       <c r="E63" s="8">
-        <f>C63-B63</f>
+        <f t="shared" si="0"/>
         <v>1.0004441719502211E-10</v>
       </c>
     </row>
@@ -7235,7 +7211,7 @@
         <v>0</v>
       </c>
       <c r="E64" s="8">
-        <f>C64-B64</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7253,7 +7229,7 @@
         <v>0</v>
       </c>
       <c r="E65" s="8">
-        <f>C65-B65</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -7271,7 +7247,7 @@
         <v>0</v>
       </c>
       <c r="E66" s="8">
-        <f>C66-B66</f>
+        <f t="shared" ref="E66:E129" si="1">C66-B66</f>
         <v>0</v>
       </c>
     </row>
@@ -7289,7 +7265,7 @@
         <v>0</v>
       </c>
       <c r="E67" s="8">
-        <f>C67-B67</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -7307,7 +7283,7 @@
         <v>0</v>
       </c>
       <c r="E68" s="8">
-        <f>C68-B68</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -7325,7 +7301,7 @@
         <v>16</v>
       </c>
       <c r="E69" s="8">
-        <f>C69-B69</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -7343,7 +7319,7 @@
         <v>16</v>
       </c>
       <c r="E70" s="8">
-        <f>C70-B70</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -7361,7 +7337,7 @@
         <v>0</v>
       </c>
       <c r="E71" s="8">
-        <f>C71-B71</f>
+        <f t="shared" si="1"/>
         <v>3.0770024750381708E-7</v>
       </c>
     </row>
@@ -7379,7 +7355,7 @@
         <v>0</v>
       </c>
       <c r="E72" s="8">
-        <f>C72-B72</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -7397,7 +7373,7 @@
         <v>0</v>
       </c>
       <c r="E73" s="8">
-        <f>C73-B73</f>
+        <f t="shared" si="1"/>
         <v>-1.1111023923149332E-7</v>
       </c>
     </row>
@@ -7415,7 +7391,7 @@
         <v>0</v>
       </c>
       <c r="E74" s="8">
-        <f>C74-B74</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -7433,7 +7409,7 @@
         <v>0</v>
       </c>
       <c r="E75" s="8">
-        <f>C75-B75</f>
+        <f t="shared" si="1"/>
         <v>1.0004441719502211E-11</v>
       </c>
     </row>
@@ -7451,7 +7427,7 @@
         <v>0</v>
       </c>
       <c r="E76" s="8">
-        <f>C76-B76</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -7469,7 +7445,7 @@
         <v>0</v>
       </c>
       <c r="E77" s="8">
-        <f>C77-B77</f>
+        <f t="shared" si="1"/>
         <v>-1.0004441719502211E-10</v>
       </c>
     </row>
@@ -7487,7 +7463,7 @@
         <v>0</v>
       </c>
       <c r="E78" s="8">
-        <f>C78-B78</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -7505,7 +7481,7 @@
         <v>0</v>
       </c>
       <c r="E79" s="8">
-        <f>C79-B79</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -7523,7 +7499,7 @@
         <v>16</v>
       </c>
       <c r="E80" s="8">
-        <f>C80-B80</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -7541,7 +7517,7 @@
         <v>0</v>
       </c>
       <c r="E81" s="8">
-        <f>C81-B81</f>
+        <f t="shared" si="1"/>
         <v>-1.9148939855995195E-7</v>
       </c>
     </row>
@@ -7559,7 +7535,7 @@
         <v>0</v>
       </c>
       <c r="E82" s="8">
-        <f>C82-B82</f>
+        <f t="shared" si="1"/>
         <v>9.558498049955233E-6</v>
       </c>
     </row>
@@ -7577,7 +7553,7 @@
         <v>0</v>
       </c>
       <c r="E83" s="8">
-        <f>C83-B83</f>
+        <f t="shared" si="1"/>
         <v>1.9603504597398569E-8</v>
       </c>
     </row>
@@ -7595,7 +7571,7 @@
         <v>0</v>
       </c>
       <c r="E84" s="8">
-        <f>C84-B84</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -7613,7 +7589,7 @@
         <v>0</v>
       </c>
       <c r="E85" s="8">
-        <f>C85-B85</f>
+        <f t="shared" si="1"/>
         <v>3.2345099043595837E-7</v>
       </c>
     </row>
@@ -7631,7 +7607,7 @@
         <v>16</v>
       </c>
       <c r="E86" s="8">
-        <f>C86-B86</f>
+        <f t="shared" si="1"/>
         <v>1.0231815394945443E-12</v>
       </c>
     </row>
@@ -7649,7 +7625,7 @@
         <v>0</v>
       </c>
       <c r="E87" s="8">
-        <f>C87-B87</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -7667,7 +7643,7 @@
         <v>0</v>
       </c>
       <c r="E88" s="8">
-        <f>C88-B88</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -7685,7 +7661,7 @@
         <v>0</v>
       </c>
       <c r="E89" s="8">
-        <f>C89-B89</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -7703,7 +7679,7 @@
         <v>0</v>
       </c>
       <c r="E90" s="7" t="e">
-        <f>C90-B90</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -7721,7 +7697,7 @@
         <v>0</v>
       </c>
       <c r="E91" s="7">
-        <f>C91-B91</f>
+        <f t="shared" si="1"/>
         <v>997.529583</v>
       </c>
     </row>
@@ -7739,7 +7715,7 @@
         <v>0</v>
       </c>
       <c r="E92" s="7">
-        <f>C92-B92</f>
+        <f t="shared" si="1"/>
         <v>1005.664817</v>
       </c>
     </row>
@@ -7757,7 +7733,7 @@
         <v>0</v>
       </c>
       <c r="E93" s="7">
-        <f>C93-B93</f>
+        <f t="shared" si="1"/>
         <v>55535.436388000002</v>
       </c>
     </row>
@@ -7772,7 +7748,7 @@
         <v>0</v>
       </c>
       <c r="E94" s="7" t="e">
-        <f>C94-B94</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -7787,7 +7763,7 @@
         <v>11</v>
       </c>
       <c r="E95" s="7" t="e">
-        <f>C95-B95</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -7802,7 +7778,7 @@
         <v>0</v>
       </c>
       <c r="E96" s="7" t="e">
-        <f>C96-B96</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -7820,7 +7796,7 @@
         <v>0</v>
       </c>
       <c r="E97" s="7">
-        <f>C97-B97</f>
+        <f t="shared" si="1"/>
         <v>2141734.6848780001</v>
       </c>
     </row>
@@ -7838,7 +7814,7 @@
         <v>0</v>
       </c>
       <c r="E98" s="7">
-        <f>C98-B98</f>
+        <f t="shared" si="1"/>
         <v>4034.2183329999998</v>
       </c>
     </row>
@@ -7853,7 +7829,7 @@
         <v>16</v>
       </c>
       <c r="E99" s="7" t="e">
-        <f>C99-B99</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -7868,7 +7844,7 @@
         <v>16</v>
       </c>
       <c r="E100" s="7" t="e">
-        <f>C100-B100</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -7883,7 +7859,7 @@
         <v>0</v>
       </c>
       <c r="E101" s="7" t="e">
-        <f>C101-B101</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -7901,7 +7877,7 @@
         <v>0</v>
       </c>
       <c r="E102" s="7">
-        <f>C102-B102</f>
+        <f t="shared" si="1"/>
         <v>125.3516947310998</v>
       </c>
     </row>
@@ -7919,7 +7895,7 @@
         <v>0</v>
       </c>
       <c r="E103" s="7">
-        <f>C103-B103</f>
+        <f t="shared" si="1"/>
         <v>105557.3500311395</v>
       </c>
     </row>
@@ -7937,7 +7913,7 @@
         <v>0</v>
       </c>
       <c r="E104" s="7">
-        <f>C104-B104</f>
+        <f t="shared" si="1"/>
         <v>3060037.4307630002</v>
       </c>
     </row>
@@ -7955,7 +7931,7 @@
         <v>0</v>
       </c>
       <c r="E105" s="7">
-        <f>C105-B105</f>
+        <f t="shared" si="1"/>
         <v>11.724138</v>
       </c>
     </row>
@@ -7973,7 +7949,7 @@
         <v>0</v>
       </c>
       <c r="E106" s="7">
-        <f>C106-B106</f>
+        <f t="shared" si="1"/>
         <v>6637.1880270000001</v>
       </c>
     </row>
@@ -7988,7 +7964,7 @@
         <v>0</v>
       </c>
       <c r="E107" s="7" t="e">
-        <f>C107-B107</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8006,7 +7982,7 @@
         <v>0</v>
       </c>
       <c r="E108" s="7">
-        <f>C108-B108</f>
+        <f t="shared" si="1"/>
         <v>5891.2265799999996</v>
       </c>
     </row>
@@ -8024,7 +8000,7 @@
         <v>0</v>
       </c>
       <c r="E109" s="7">
-        <f>C109-B109</f>
+        <f t="shared" si="1"/>
         <v>3846.358667</v>
       </c>
     </row>
@@ -8039,7 +8015,7 @@
         <v>0</v>
       </c>
       <c r="E110" s="7" t="e">
-        <f>C110-B110</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8054,7 +8030,7 @@
         <v>16</v>
       </c>
       <c r="E111" s="7" t="e">
-        <f>C111-B111</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8069,7 +8045,7 @@
         <v>16</v>
       </c>
       <c r="E112" s="7" t="e">
-        <f>C112-B112</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8084,7 +8060,7 @@
         <v>0</v>
       </c>
       <c r="E113" s="7" t="e">
-        <f>C113-B113</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8099,7 +8075,7 @@
         <v>16</v>
       </c>
       <c r="E114" s="7" t="e">
-        <f>C114-B114</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8117,7 +8093,7 @@
         <v>0</v>
       </c>
       <c r="E115" s="7">
-        <f>C115-B115</f>
+        <f t="shared" si="1"/>
         <v>269.25158699999997</v>
       </c>
     </row>
@@ -8135,7 +8111,7 @@
         <v>0</v>
       </c>
       <c r="E116" s="7">
-        <f>C116-B116</f>
+        <f t="shared" si="1"/>
         <v>120</v>
       </c>
     </row>
@@ -8153,7 +8129,7 @@
         <v>0</v>
       </c>
       <c r="E117" s="7">
-        <f>C117-B117</f>
+        <f t="shared" si="1"/>
         <v>332.42272700000001</v>
       </c>
     </row>
@@ -8171,7 +8147,7 @@
         <v>0</v>
       </c>
       <c r="E118" s="7">
-        <f>C118-B118</f>
+        <f t="shared" si="1"/>
         <v>12425.583005</v>
       </c>
     </row>
@@ -8189,7 +8165,7 @@
         <v>16</v>
       </c>
       <c r="E119" s="7">
-        <f>C119-B119</f>
+        <f t="shared" si="1"/>
         <v>12229.625787999999</v>
       </c>
     </row>
@@ -8207,7 +8183,7 @@
         <v>16</v>
       </c>
       <c r="E120" s="7">
-        <f>C120-B120</f>
+        <f t="shared" si="1"/>
         <v>80.182402608696009</v>
       </c>
     </row>
@@ -8225,7 +8201,7 @@
         <v>0</v>
       </c>
       <c r="E121" s="7">
-        <f>C121-B121</f>
+        <f t="shared" si="1"/>
         <v>17.8587085714286</v>
       </c>
     </row>
@@ -8240,7 +8216,7 @@
         <v>16</v>
       </c>
       <c r="E122" s="7" t="e">
-        <f>C122-B122</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8258,7 +8234,7 @@
         <v>0</v>
       </c>
       <c r="E123" s="7">
-        <f>C123-B123</f>
+        <f t="shared" si="1"/>
         <v>1754946.8636380001</v>
       </c>
     </row>
@@ -8276,7 +8252,7 @@
         <v>16</v>
       </c>
       <c r="E124" s="7">
-        <f>C124-B124</f>
+        <f t="shared" si="1"/>
         <v>1744591.692942</v>
       </c>
     </row>
@@ -8294,7 +8270,7 @@
         <v>0</v>
       </c>
       <c r="E125" s="7">
-        <f>C125-B125</f>
+        <f t="shared" si="1"/>
         <v>2400.0000002734014</v>
       </c>
     </row>
@@ -8312,7 +8288,7 @@
         <v>0</v>
       </c>
       <c r="E126" s="7">
-        <f>C126-B126</f>
+        <f t="shared" si="1"/>
         <v>482102.77406499401</v>
       </c>
     </row>
@@ -8330,7 +8306,7 @@
         <v>0</v>
       </c>
       <c r="E127" s="7">
-        <f>C127-B127</f>
+        <f t="shared" si="1"/>
         <v>6556066.0683150003</v>
       </c>
     </row>
@@ -8345,7 +8321,7 @@
         <v>16</v>
       </c>
       <c r="E128" s="7" t="e">
-        <f>C128-B128</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8363,7 +8339,7 @@
         <v>0</v>
       </c>
       <c r="E129" s="7" t="e">
-        <f>C129-B129</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8381,7 +8357,7 @@
         <v>0</v>
       </c>
       <c r="E130" s="7" t="e">
-        <f>C130-B130</f>
+        <f t="shared" ref="E130:E193" si="2">C130-B130</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8399,7 +8375,7 @@
         <v>0</v>
       </c>
       <c r="E131" s="7">
-        <f>C131-B131</f>
+        <f t="shared" si="2"/>
         <v>1075.247691</v>
       </c>
     </row>
@@ -8414,7 +8390,7 @@
         <v>0</v>
       </c>
       <c r="E132" s="7" t="e">
-        <f>C132-B132</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8429,7 +8405,7 @@
         <v>0</v>
       </c>
       <c r="E133" s="7" t="e">
-        <f>C133-B133</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8444,7 +8420,7 @@
         <v>16</v>
       </c>
       <c r="E134" s="7" t="e">
-        <f>C134-B134</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8459,7 +8435,7 @@
         <v>0</v>
       </c>
       <c r="E135" s="7" t="e">
-        <f>C135-B135</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8477,7 +8453,7 @@
         <v>0</v>
       </c>
       <c r="E136" s="7">
-        <f>C136-B136</f>
+        <f t="shared" si="2"/>
         <v>100002400</v>
       </c>
     </row>
@@ -8495,7 +8471,7 @@
         <v>0</v>
       </c>
       <c r="E137" s="7">
-        <f>C137-B137</f>
+        <f t="shared" si="2"/>
         <v>918330.72415225022</v>
       </c>
     </row>
@@ -8513,7 +8489,7 @@
         <v>0</v>
       </c>
       <c r="E138" s="7">
-        <f>C138-B138</f>
+        <f t="shared" si="2"/>
         <v>823668.34776423033</v>
       </c>
     </row>
@@ -8528,7 +8504,7 @@
         <v>16</v>
       </c>
       <c r="E139" s="7" t="e">
-        <f>C139-B139</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8546,7 +8522,7 @@
         <v>16</v>
       </c>
       <c r="E140" s="7">
-        <f>C140-B140</f>
+        <f t="shared" si="2"/>
         <v>1916516.1466591004</v>
       </c>
     </row>
@@ -8561,7 +8537,7 @@
         <v>0</v>
       </c>
       <c r="E141" s="7" t="e">
-        <f>C141-B141</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8576,7 +8552,7 @@
         <v>16</v>
       </c>
       <c r="E142" s="7" t="e">
-        <f>C142-B142</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8591,7 +8567,7 @@
         <v>0</v>
       </c>
       <c r="E143" s="7" t="e">
-        <f>C143-B143</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8606,7 +8582,7 @@
         <v>16</v>
       </c>
       <c r="E144" s="7" t="e">
-        <f>C144-B144</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8621,7 +8597,7 @@
         <v>16</v>
       </c>
       <c r="E145" s="7" t="e">
-        <f>C145-B145</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8636,7 +8612,7 @@
         <v>0</v>
       </c>
       <c r="E146" s="7" t="e">
-        <f>C146-B146</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8651,7 +8627,7 @@
         <v>16</v>
       </c>
       <c r="E147" s="7" t="e">
-        <f>C147-B147</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8666,7 +8642,7 @@
         <v>0</v>
       </c>
       <c r="E148" s="7" t="e">
-        <f>C148-B148</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8681,7 +8657,7 @@
         <v>0</v>
       </c>
       <c r="E149" s="7" t="e">
-        <f>C149-B149</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8696,7 +8672,7 @@
         <v>0</v>
       </c>
       <c r="E150" s="7" t="e">
-        <f>C150-B150</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8714,7 +8690,7 @@
         <v>0</v>
       </c>
       <c r="E151" s="7">
-        <f>C151-B151</f>
+        <f t="shared" si="2"/>
         <v>388573315.50960797</v>
       </c>
     </row>
@@ -8732,7 +8708,7 @@
         <v>0</v>
       </c>
       <c r="E152" s="7">
-        <f>C152-B152</f>
+        <f t="shared" si="2"/>
         <v>386421293.20891899</v>
       </c>
     </row>
@@ -8750,7 +8726,7 @@
         <v>0</v>
       </c>
       <c r="E153" s="7">
-        <f>C153-B153</f>
+        <f t="shared" si="2"/>
         <v>348385.34655100002</v>
       </c>
     </row>
@@ -8765,7 +8741,7 @@
         <v>11</v>
       </c>
       <c r="E154" s="7" t="e">
-        <f>C154-B154</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8780,7 +8756,7 @@
         <v>0</v>
       </c>
       <c r="E155" s="7" t="e">
-        <f>C155-B155</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8795,7 +8771,7 @@
         <v>0</v>
       </c>
       <c r="E156" s="7" t="e">
-        <f>C156-B156</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8810,7 +8786,7 @@
         <v>0</v>
       </c>
       <c r="E157" s="7" t="e">
-        <f>C157-B157</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8825,7 +8801,7 @@
         <v>0</v>
       </c>
       <c r="E158" s="7" t="e">
-        <f>C158-B158</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8840,7 +8816,7 @@
         <v>0</v>
       </c>
       <c r="E159" s="7" t="e">
-        <f>C159-B159</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8858,7 +8834,7 @@
         <v>0</v>
       </c>
       <c r="E160" s="7" t="e">
-        <f>C160-B160</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8876,7 +8852,7 @@
         <v>0</v>
       </c>
       <c r="E161" s="7">
-        <f>C161-B161</f>
+        <f t="shared" si="2"/>
         <v>193774.753707</v>
       </c>
     </row>
@@ -8891,7 +8867,7 @@
         <v>16</v>
       </c>
       <c r="E162" s="7" t="e">
-        <f>C162-B162</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8909,7 +8885,7 @@
         <v>0</v>
       </c>
       <c r="E163" s="7" t="e">
-        <f>C163-B163</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8924,7 +8900,7 @@
         <v>0</v>
       </c>
       <c r="E164" s="7" t="e">
-        <f>C164-B164</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8942,7 +8918,7 @@
         <v>0</v>
       </c>
       <c r="E165" s="7">
-        <f>C165-B165</f>
+        <f t="shared" si="2"/>
         <v>29756289.590557933</v>
       </c>
     </row>
@@ -8957,7 +8933,7 @@
         <v>16</v>
       </c>
       <c r="E166" s="7" t="e">
-        <f>C166-B166</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8975,7 +8951,7 @@
         <v>0</v>
       </c>
       <c r="E167" s="7" t="e">
-        <f>C167-B167</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -8990,7 +8966,7 @@
         <v>0</v>
       </c>
       <c r="E168" s="7" t="e">
-        <f>C168-B168</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9005,7 +8981,7 @@
         <v>0</v>
       </c>
       <c r="E169" s="7" t="e">
-        <f>C169-B169</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9020,7 +8996,7 @@
         <v>16</v>
       </c>
       <c r="E170" s="7" t="e">
-        <f>C170-B170</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9035,7 +9011,7 @@
         <v>0</v>
       </c>
       <c r="E171" s="7" t="e">
-        <f>C171-B171</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9050,7 +9026,7 @@
         <v>0</v>
       </c>
       <c r="E172" s="7" t="e">
-        <f>C172-B172</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9065,7 +9041,7 @@
         <v>0</v>
       </c>
       <c r="E173" s="7" t="e">
-        <f>C173-B173</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9080,7 +9056,7 @@
         <v>16</v>
       </c>
       <c r="E174" s="7" t="e">
-        <f>C174-B174</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9095,7 +9071,7 @@
         <v>16</v>
       </c>
       <c r="E175" s="7" t="e">
-        <f>C175-B175</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9110,7 +9086,7 @@
         <v>16</v>
       </c>
       <c r="E176" s="7" t="e">
-        <f>C176-B176</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9125,7 +9101,7 @@
         <v>16</v>
       </c>
       <c r="E177" s="7" t="e">
-        <f>C177-B177</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9140,7 +9116,7 @@
         <v>0</v>
       </c>
       <c r="E178" s="7" t="e">
-        <f>C178-B178</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9155,7 +9131,7 @@
         <v>0</v>
       </c>
       <c r="E179" s="7" t="e">
-        <f>C179-B179</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9173,7 +9149,7 @@
         <v>16</v>
       </c>
       <c r="E180" s="7">
-        <f>C180-B180</f>
+        <f t="shared" si="2"/>
         <v>465</v>
       </c>
     </row>
@@ -9188,7 +9164,7 @@
         <v>16</v>
       </c>
       <c r="E181" s="7" t="e">
-        <f>C181-B181</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9203,7 +9179,7 @@
         <v>0</v>
       </c>
       <c r="E182" s="7" t="e">
-        <f>C182-B182</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9218,7 +9194,7 @@
         <v>16</v>
       </c>
       <c r="E183" s="7" t="e">
-        <f>C183-B183</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9233,7 +9209,7 @@
         <v>0</v>
       </c>
       <c r="E184" s="7" t="e">
-        <f>C184-B184</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9248,7 +9224,7 @@
         <v>0</v>
       </c>
       <c r="E185" s="7" t="e">
-        <f>C185-B185</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9266,7 +9242,7 @@
         <v>0</v>
       </c>
       <c r="E186" s="7">
-        <f>C186-B186</f>
+        <f t="shared" si="2"/>
         <v>388.55239999999998</v>
       </c>
     </row>
@@ -9281,7 +9257,7 @@
         <v>16</v>
       </c>
       <c r="E187" s="7" t="e">
-        <f>C187-B187</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9299,7 +9275,7 @@
         <v>0</v>
       </c>
       <c r="E188" s="7">
-        <f>C188-B188</f>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
     </row>
@@ -9317,7 +9293,7 @@
         <v>0</v>
       </c>
       <c r="E189" s="7">
-        <f>C189-B189</f>
+        <f t="shared" si="2"/>
         <v>29624.693694000001</v>
       </c>
     </row>
@@ -9335,7 +9311,7 @@
         <v>0</v>
       </c>
       <c r="E190" s="7">
-        <f>C190-B190</f>
+        <f t="shared" si="2"/>
         <v>429</v>
       </c>
     </row>
@@ -9353,7 +9329,7 @@
         <v>0</v>
       </c>
       <c r="E191" s="7">
-        <f>C191-B191</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -9371,7 +9347,7 @@
         <v>0</v>
       </c>
       <c r="E192" s="7">
-        <f>C192-B192</f>
+        <f t="shared" si="2"/>
         <v>6.1507350000000001</v>
       </c>
     </row>
@@ -9389,7 +9365,7 @@
         <v>0</v>
       </c>
       <c r="E193" s="7">
-        <f>C193-B193</f>
+        <f t="shared" si="2"/>
         <v>2.4120712941176481</v>
       </c>
     </row>
@@ -9404,7 +9380,7 @@
         <v>0</v>
       </c>
       <c r="E194" s="7" t="e">
-        <f>C194-B194</f>
+        <f t="shared" ref="E194:E257" si="3">C194-B194</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9419,7 +9395,7 @@
         <v>0</v>
       </c>
       <c r="E195" s="7" t="e">
-        <f>C195-B195</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9434,7 +9410,7 @@
         <v>0</v>
       </c>
       <c r="E196" s="7" t="e">
-        <f>C196-B196</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9449,7 +9425,7 @@
         <v>0</v>
       </c>
       <c r="E197" s="7" t="e">
-        <f>C197-B197</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9464,7 +9440,7 @@
         <v>0</v>
       </c>
       <c r="E198" s="7" t="e">
-        <f>C198-B198</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9482,7 +9458,7 @@
         <v>0</v>
       </c>
       <c r="E199" s="7">
-        <f>C199-B199</f>
+        <f t="shared" si="3"/>
         <v>1089619.547762725</v>
       </c>
     </row>
@@ -9500,7 +9476,7 @@
         <v>0</v>
       </c>
       <c r="E200" s="7">
-        <f>C200-B200</f>
+        <f t="shared" si="3"/>
         <v>83</v>
       </c>
     </row>
@@ -9515,7 +9491,7 @@
         <v>0</v>
       </c>
       <c r="E201" s="7" t="e">
-        <f>C201-B201</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9533,7 +9509,7 @@
         <v>0</v>
       </c>
       <c r="E202" s="7">
-        <f>C202-B202</f>
+        <f t="shared" si="3"/>
         <v>5134.8138300000001</v>
       </c>
     </row>
@@ -9551,7 +9527,7 @@
         <v>0</v>
       </c>
       <c r="E203" s="7">
-        <f>C203-B203</f>
+        <f t="shared" si="3"/>
         <v>234</v>
       </c>
     </row>
@@ -9566,7 +9542,7 @@
         <v>0</v>
       </c>
       <c r="E204" s="7" t="e">
-        <f>C204-B204</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9581,7 +9557,7 @@
         <v>0</v>
       </c>
       <c r="E205" s="7" t="e">
-        <f>C205-B205</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9599,7 +9575,7 @@
         <v>11</v>
       </c>
       <c r="E206" s="7">
-        <f>C206-B206</f>
+        <f t="shared" si="3"/>
         <v>280</v>
       </c>
     </row>
@@ -9617,7 +9593,7 @@
         <v>0</v>
       </c>
       <c r="E207" s="7" t="e">
-        <f>C207-B207</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9632,7 +9608,7 @@
         <v>0</v>
       </c>
       <c r="E208" s="7" t="e">
-        <f>C208-B208</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9647,7 +9623,7 @@
         <v>0</v>
       </c>
       <c r="E209" s="7" t="e">
-        <f>C209-B209</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9662,7 +9638,7 @@
         <v>0</v>
       </c>
       <c r="E210" s="7" t="e">
-        <f>C210-B210</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9677,7 +9653,7 @@
         <v>0</v>
       </c>
       <c r="E211" s="7" t="e">
-        <f>C211-B211</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9692,7 +9668,7 @@
         <v>0</v>
       </c>
       <c r="E212" s="7" t="e">
-        <f>C212-B212</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9710,7 +9686,7 @@
         <v>0</v>
       </c>
       <c r="E213" s="7">
-        <f>C213-B213</f>
+        <f t="shared" si="3"/>
         <v>23.26</v>
       </c>
     </row>
@@ -9728,7 +9704,7 @@
         <v>0</v>
       </c>
       <c r="E214" s="7">
-        <f>C214-B214</f>
+        <f t="shared" si="3"/>
         <v>26.203596000000001</v>
       </c>
     </row>
@@ -9743,7 +9719,7 @@
         <v>0</v>
       </c>
       <c r="E215" s="7" t="e">
-        <f>C215-B215</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9758,7 +9734,7 @@
         <v>0</v>
       </c>
       <c r="E216" s="7" t="e">
-        <f>C216-B216</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9773,7 +9749,7 @@
         <v>0</v>
       </c>
       <c r="E217" s="7" t="e">
-        <f>C217-B217</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9788,7 +9764,7 @@
         <v>0</v>
       </c>
       <c r="E218" s="7" t="e">
-        <f>C218-B218</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9803,7 +9779,7 @@
         <v>0</v>
       </c>
       <c r="E219" s="7" t="e">
-        <f>C219-B219</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9818,7 +9794,7 @@
         <v>0</v>
       </c>
       <c r="E220" s="7" t="e">
-        <f>C220-B220</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9833,7 +9809,7 @@
         <v>0</v>
       </c>
       <c r="E221" s="7" t="e">
-        <f>C221-B221</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9848,7 +9824,7 @@
         <v>16</v>
       </c>
       <c r="E222" s="7" t="e">
-        <f>C222-B222</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9863,7 +9839,7 @@
         <v>0</v>
       </c>
       <c r="E223" s="7" t="e">
-        <f>C223-B223</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9878,7 +9854,7 @@
         <v>0</v>
       </c>
       <c r="E224" s="7" t="e">
-        <f>C224-B224</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9896,7 +9872,7 @@
         <v>0</v>
       </c>
       <c r="E225" s="7">
-        <f>C225-B225</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
     </row>
@@ -9911,7 +9887,7 @@
         <v>0</v>
       </c>
       <c r="E226" s="7" t="e">
-        <f>C226-B226</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9929,7 +9905,7 @@
         <v>16</v>
       </c>
       <c r="E227" s="7">
-        <f>C227-B227</f>
+        <f t="shared" si="3"/>
         <v>9.3400693892001527</v>
       </c>
     </row>
@@ -9944,7 +9920,7 @@
         <v>16</v>
       </c>
       <c r="E228" s="7" t="e">
-        <f>C228-B228</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9959,7 +9935,7 @@
         <v>0</v>
       </c>
       <c r="E229" s="7" t="e">
-        <f>C229-B229</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9974,7 +9950,7 @@
         <v>0</v>
       </c>
       <c r="E230" s="7" t="e">
-        <f>C230-B230</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -9992,7 +9968,7 @@
         <v>0</v>
       </c>
       <c r="E231" s="7">
-        <f>C231-B231</f>
+        <f t="shared" si="3"/>
         <v>11.724138</v>
       </c>
     </row>
@@ -10007,7 +9983,7 @@
         <v>0</v>
       </c>
       <c r="E232" s="7" t="e">
-        <f>C232-B232</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10022,7 +9998,7 @@
         <v>0</v>
       </c>
       <c r="E233" s="7" t="e">
-        <f>C233-B233</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10037,7 +10013,7 @@
         <v>0</v>
       </c>
       <c r="E234" s="7" t="e">
-        <f>C234-B234</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10052,7 +10028,7 @@
         <v>11</v>
       </c>
       <c r="E235" s="7" t="e">
-        <f>C235-B235</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10070,7 +10046,7 @@
         <v>16</v>
       </c>
       <c r="E236" s="7">
-        <f>C236-B236</f>
+        <f t="shared" si="3"/>
         <v>361.93902200000002</v>
       </c>
     </row>
@@ -10088,7 +10064,7 @@
         <v>0</v>
       </c>
       <c r="E237" s="7">
-        <f>C237-B237</f>
+        <f t="shared" si="3"/>
         <v>13224.197610294117</v>
       </c>
     </row>
@@ -10103,7 +10079,7 @@
         <v>16</v>
       </c>
       <c r="E238" s="7" t="e">
-        <f>C238-B238</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10118,7 +10094,7 @@
         <v>0</v>
       </c>
       <c r="E239" s="7" t="e">
-        <f>C239-B239</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10133,7 +10109,7 @@
         <v>0</v>
       </c>
       <c r="E240" s="7" t="e">
-        <f>C240-B240</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10148,7 +10124,7 @@
         <v>0</v>
       </c>
       <c r="E241" s="7" t="e">
-        <f>C241-B241</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10166,7 +10142,7 @@
         <v>11</v>
       </c>
       <c r="E242" s="7">
-        <f>C242-B242</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -10184,7 +10160,7 @@
         <v>0</v>
       </c>
       <c r="E243" s="7">
-        <f>C243-B243</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -10199,7 +10175,7 @@
         <v>0</v>
       </c>
       <c r="E244" s="7" t="e">
-        <f>C244-B244</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10217,7 +10193,7 @@
         <v>11</v>
       </c>
       <c r="E245" s="7">
-        <f>C245-B245</f>
+        <f t="shared" si="3"/>
         <v>1700</v>
       </c>
     </row>
@@ -10235,7 +10211,7 @@
         <v>11</v>
       </c>
       <c r="E246" s="7">
-        <f>C246-B246</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
@@ -10250,7 +10226,7 @@
         <v>0</v>
       </c>
       <c r="E247" s="7" t="e">
-        <f>C247-B247</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10268,7 +10244,7 @@
         <v>11</v>
       </c>
       <c r="E248" s="7">
-        <f>C248-B248</f>
+        <f t="shared" si="3"/>
         <v>5833.8</v>
       </c>
     </row>
@@ -10286,7 +10262,7 @@
         <v>11</v>
       </c>
       <c r="E249" s="7">
-        <f>C249-B249</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
@@ -10301,7 +10277,7 @@
         <v>16</v>
       </c>
       <c r="E250" s="7" t="e">
-        <f>C250-B250</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10319,7 +10295,7 @@
         <v>0</v>
       </c>
       <c r="E251" s="7">
-        <f>C251-B251</f>
+        <f t="shared" si="3"/>
         <v>6153</v>
       </c>
     </row>
@@ -10334,7 +10310,7 @@
         <v>16</v>
       </c>
       <c r="E252" s="7" t="e">
-        <f>C252-B252</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10349,7 +10325,7 @@
         <v>16</v>
       </c>
       <c r="E253" s="7" t="e">
-        <f>C253-B253</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10364,7 +10340,7 @@
         <v>16</v>
       </c>
       <c r="E254" s="7" t="e">
-        <f>C254-B254</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10379,7 +10355,7 @@
         <v>16</v>
       </c>
       <c r="E255" s="7" t="e">
-        <f>C255-B255</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10394,7 +10370,7 @@
         <v>16</v>
       </c>
       <c r="E256" s="7" t="e">
-        <f>C256-B256</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10409,7 +10385,7 @@
         <v>16</v>
       </c>
       <c r="E257" s="7" t="e">
-        <f>C257-B257</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10424,7 +10400,7 @@
         <v>0</v>
       </c>
       <c r="E258" s="7" t="e">
-        <f>C258-B258</f>
+        <f t="shared" ref="E258:E321" si="4">C258-B258</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10442,7 +10418,7 @@
         <v>0</v>
       </c>
       <c r="E259" s="7">
-        <f>C259-B259</f>
+        <f t="shared" si="4"/>
         <v>4.5999999999999996</v>
       </c>
     </row>
@@ -10457,7 +10433,7 @@
         <v>11</v>
       </c>
       <c r="E260" s="7" t="e">
-        <f>C260-B260</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10472,7 +10448,7 @@
         <v>16</v>
       </c>
       <c r="E261" s="7" t="e">
-        <f>C261-B261</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10487,7 +10463,7 @@
         <v>16</v>
       </c>
       <c r="E262" s="7" t="e">
-        <f>C262-B262</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10502,7 +10478,7 @@
         <v>16</v>
       </c>
       <c r="E263" s="7" t="e">
-        <f>C263-B263</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10517,7 +10493,7 @@
         <v>16</v>
       </c>
       <c r="E264" s="7" t="e">
-        <f>C264-B264</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10532,7 +10508,7 @@
         <v>0</v>
       </c>
       <c r="E265" s="7" t="e">
-        <f>C265-B265</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10547,7 +10523,7 @@
         <v>16</v>
       </c>
       <c r="E266" s="7" t="e">
-        <f>C266-B266</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10565,7 +10541,7 @@
         <v>0</v>
       </c>
       <c r="E267" s="7">
-        <f>C267-B267</f>
+        <f t="shared" si="4"/>
         <v>6.3048019999999996</v>
       </c>
     </row>
@@ -10580,7 +10556,7 @@
         <v>16</v>
       </c>
       <c r="E268" s="7" t="e">
-        <f>C268-B268</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10595,7 +10571,7 @@
         <v>16</v>
       </c>
       <c r="E269" s="7" t="e">
-        <f>C269-B269</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10610,7 +10586,7 @@
         <v>16</v>
       </c>
       <c r="E270" s="7" t="e">
-        <f>C270-B270</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10625,7 +10601,7 @@
         <v>0</v>
       </c>
       <c r="E271" s="7" t="e">
-        <f>C271-B271</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10640,7 +10616,7 @@
         <v>0</v>
       </c>
       <c r="E272" s="7" t="e">
-        <f>C272-B272</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10655,7 +10631,7 @@
         <v>0</v>
       </c>
       <c r="E273" s="7" t="e">
-        <f>C273-B273</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10670,7 +10646,7 @@
         <v>0</v>
       </c>
       <c r="E274" s="7" t="e">
-        <f>C274-B274</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10685,7 +10661,7 @@
         <v>0</v>
       </c>
       <c r="E275" s="7" t="e">
-        <f>C275-B275</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10700,7 +10676,7 @@
         <v>0</v>
       </c>
       <c r="E276" s="7" t="e">
-        <f>C276-B276</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10715,7 +10691,7 @@
         <v>11</v>
       </c>
       <c r="E277" s="7" t="e">
-        <f>C277-B277</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10730,7 +10706,7 @@
         <v>16</v>
       </c>
       <c r="E278" s="7" t="e">
-        <f>C278-B278</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10748,7 +10724,7 @@
         <v>0</v>
       </c>
       <c r="E279" s="7">
-        <f>C279-B279</f>
+        <f t="shared" si="4"/>
         <v>381575.49261800002</v>
       </c>
     </row>
@@ -10766,7 +10742,7 @@
         <v>0</v>
       </c>
       <c r="E280" s="7">
-        <f>C280-B280</f>
+        <f t="shared" si="4"/>
         <v>384870.29177809798</v>
       </c>
     </row>
@@ -10784,7 +10760,7 @@
         <v>0</v>
       </c>
       <c r="E281" s="7">
-        <f>C281-B281</f>
+        <f t="shared" si="4"/>
         <v>0.48726136476443038</v>
       </c>
     </row>
@@ -10799,7 +10775,7 @@
         <v>0</v>
       </c>
       <c r="E282" s="7" t="e">
-        <f>C282-B282</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10814,7 +10790,7 @@
         <v>0</v>
       </c>
       <c r="E283" s="7" t="e">
-        <f>C283-B283</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10829,7 +10805,7 @@
         <v>0</v>
       </c>
       <c r="E284" s="7" t="e">
-        <f>C284-B284</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10844,7 +10820,7 @@
         <v>0</v>
       </c>
       <c r="E285" s="7" t="e">
-        <f>C285-B285</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10862,7 +10838,7 @@
         <v>0</v>
       </c>
       <c r="E286" s="7">
-        <f>C286-B286</f>
+        <f t="shared" si="4"/>
         <v>3016.9443540000002</v>
       </c>
     </row>
@@ -10880,7 +10856,7 @@
         <v>0</v>
       </c>
       <c r="E287" s="7" t="e">
-        <f>C287-B287</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10898,7 +10874,7 @@
         <v>0</v>
       </c>
       <c r="E288" s="7">
-        <f>C288-B288</f>
+        <f t="shared" si="4"/>
         <v>3116.4295120000002</v>
       </c>
     </row>
@@ -10913,7 +10889,7 @@
         <v>0</v>
       </c>
       <c r="E289" s="7" t="e">
-        <f>C289-B289</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10928,7 +10904,7 @@
         <v>0</v>
       </c>
       <c r="E290" s="7" t="e">
-        <f>C290-B290</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10943,7 +10919,7 @@
         <v>0</v>
       </c>
       <c r="E291" s="7" t="e">
-        <f>C291-B291</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10961,7 +10937,7 @@
         <v>0</v>
       </c>
       <c r="E292" s="7">
-        <f>C292-B292</f>
+        <f t="shared" si="4"/>
         <v>838185.66189719737</v>
       </c>
     </row>
@@ -10976,7 +10952,7 @@
         <v>0</v>
       </c>
       <c r="E293" s="7" t="e">
-        <f>C293-B293</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -10991,7 +10967,7 @@
         <v>0</v>
       </c>
       <c r="E294" s="7" t="e">
-        <f>C294-B294</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11006,7 +10982,7 @@
         <v>0</v>
       </c>
       <c r="E295" s="7" t="e">
-        <f>C295-B295</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11021,7 +10997,7 @@
         <v>0</v>
       </c>
       <c r="E296" s="7" t="e">
-        <f>C296-B296</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11036,7 +11012,7 @@
         <v>0</v>
       </c>
       <c r="E297" s="7" t="e">
-        <f>C297-B297</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11051,7 +11027,7 @@
         <v>16</v>
       </c>
       <c r="E298" s="7" t="e">
-        <f>C298-B298</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11066,7 +11042,7 @@
         <v>16</v>
       </c>
       <c r="E299" s="7" t="e">
-        <f>C299-B299</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11081,7 +11057,7 @@
         <v>16</v>
       </c>
       <c r="E300" s="7" t="e">
-        <f>C300-B300</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11096,7 +11072,7 @@
         <v>16</v>
       </c>
       <c r="E301" s="7" t="e">
-        <f>C301-B301</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11114,7 +11090,7 @@
         <v>0</v>
       </c>
       <c r="E302" s="7">
-        <f>C302-B302</f>
+        <f t="shared" si="4"/>
         <v>2588.28359539249</v>
       </c>
     </row>
@@ -11129,7 +11105,7 @@
         <v>0</v>
       </c>
       <c r="E303" s="7" t="e">
-        <f>C303-B303</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11144,7 +11120,7 @@
         <v>16</v>
       </c>
       <c r="E304" s="7" t="e">
-        <f>C304-B304</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11159,7 +11135,7 @@
         <v>16</v>
       </c>
       <c r="E305" s="7" t="e">
-        <f>C305-B305</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11177,7 +11153,7 @@
         <v>0</v>
       </c>
       <c r="E306" s="7">
-        <f>C306-B306</f>
+        <f t="shared" si="4"/>
         <v>8350.1994680000007</v>
       </c>
     </row>
@@ -11195,7 +11171,7 @@
         <v>0</v>
       </c>
       <c r="E307" s="7">
-        <f>C307-B307</f>
+        <f t="shared" si="4"/>
         <v>7515.2710290000005</v>
       </c>
     </row>
@@ -11213,7 +11189,7 @@
         <v>0</v>
       </c>
       <c r="E308" s="7">
-        <f>C308-B308</f>
+        <f t="shared" si="4"/>
         <v>9024.2054059999991</v>
       </c>
     </row>
@@ -11228,7 +11204,7 @@
         <v>16</v>
       </c>
       <c r="E309" s="7" t="e">
-        <f>C309-B309</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11246,7 +11222,7 @@
         <v>0</v>
       </c>
       <c r="E310" s="7">
-        <f>C310-B310</f>
+        <f t="shared" si="4"/>
         <v>11097.127677</v>
       </c>
     </row>
@@ -11261,7 +11237,7 @@
         <v>16</v>
       </c>
       <c r="E311" s="7" t="e">
-        <f>C311-B311</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11279,7 +11255,7 @@
         <v>0</v>
       </c>
       <c r="E312" s="7">
-        <f>C312-B312</f>
+        <f t="shared" si="4"/>
         <v>0.99986953174940041</v>
       </c>
     </row>
@@ -11294,7 +11270,7 @@
         <v>0</v>
       </c>
       <c r="E313" s="7" t="e">
-        <f>C313-B313</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11309,7 +11285,7 @@
         <v>0</v>
       </c>
       <c r="E314" s="7" t="e">
-        <f>C314-B314</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11324,7 +11300,7 @@
         <v>0</v>
       </c>
       <c r="E315" s="7" t="e">
-        <f>C315-B315</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11339,7 +11315,7 @@
         <v>0</v>
       </c>
       <c r="E316" s="7" t="e">
-        <f>C316-B316</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11354,7 +11330,7 @@
         <v>16</v>
       </c>
       <c r="E317" s="7" t="e">
-        <f>C317-B317</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11369,7 +11345,7 @@
         <v>16</v>
       </c>
       <c r="E318" s="7" t="e">
-        <f>C318-B318</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11384,7 +11360,7 @@
         <v>16</v>
       </c>
       <c r="E319" s="7" t="e">
-        <f>C319-B319</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11402,7 +11378,7 @@
         <v>16</v>
       </c>
       <c r="E320" s="7">
-        <f>C320-B320</f>
+        <f t="shared" si="4"/>
         <v>788.89065500000004</v>
       </c>
     </row>
@@ -11420,7 +11396,7 @@
         <v>0</v>
       </c>
       <c r="E321" s="7">
-        <f>C321-B321</f>
+        <f t="shared" si="4"/>
         <v>8364.0407450000002</v>
       </c>
     </row>
@@ -11438,7 +11414,7 @@
         <v>16</v>
       </c>
       <c r="E322" s="7">
-        <f>C322-B322</f>
+        <f t="shared" ref="E322:E362" si="5">C322-B322</f>
         <v>10347.381087</v>
       </c>
     </row>
@@ -11456,7 +11432,7 @@
         <v>0</v>
       </c>
       <c r="E323" s="7">
-        <f>C323-B323</f>
+        <f t="shared" si="5"/>
         <v>123.02865634809302</v>
       </c>
     </row>
@@ -11474,7 +11450,7 @@
         <v>0</v>
       </c>
       <c r="E324" s="7" t="e">
-        <f>C324-B324</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11489,7 +11465,7 @@
         <v>16</v>
       </c>
       <c r="E325" s="7" t="e">
-        <f>C325-B325</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11504,7 +11480,7 @@
         <v>0</v>
       </c>
       <c r="E326" s="7" t="e">
-        <f>C326-B326</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11522,7 +11498,7 @@
         <v>16</v>
       </c>
       <c r="E327" s="7">
-        <f>C327-B327</f>
+        <f t="shared" si="5"/>
         <v>5003432.6679425007</v>
       </c>
     </row>
@@ -11537,7 +11513,7 @@
         <v>16</v>
       </c>
       <c r="E328" s="7" t="e">
-        <f>C328-B328</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11552,7 +11528,7 @@
         <v>16</v>
       </c>
       <c r="E329" s="7" t="e">
-        <f>C329-B329</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11567,7 +11543,7 @@
         <v>16</v>
       </c>
       <c r="E330" s="7" t="e">
-        <f>C330-B330</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11582,7 +11558,7 @@
         <v>16</v>
       </c>
       <c r="E331" s="7" t="e">
-        <f>C331-B331</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11600,7 +11576,7 @@
         <v>0</v>
       </c>
       <c r="E332" s="7" t="e">
-        <f>C332-B332</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11618,7 +11594,7 @@
         <v>0</v>
       </c>
       <c r="E333" s="7">
-        <f>C333-B333</f>
+        <f t="shared" si="5"/>
         <v>593789.15769699216</v>
       </c>
     </row>
@@ -11633,7 +11609,7 @@
         <v>16</v>
       </c>
       <c r="E334" s="7" t="e">
-        <f>C334-B334</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11648,7 +11624,7 @@
         <v>16</v>
       </c>
       <c r="E335" s="7" t="e">
-        <f>C335-B335</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11663,7 +11639,7 @@
         <v>0</v>
       </c>
       <c r="E336" s="7" t="e">
-        <f>C336-B336</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11678,7 +11654,7 @@
         <v>16</v>
       </c>
       <c r="E337" s="7" t="e">
-        <f>C337-B337</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11693,7 +11669,7 @@
         <v>16</v>
       </c>
       <c r="E338" s="7" t="e">
-        <f>C338-B338</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11711,7 +11687,7 @@
         <v>0</v>
       </c>
       <c r="E339" s="7">
-        <f>C339-B339</f>
+        <f t="shared" si="5"/>
         <v>334.49685799999997</v>
       </c>
     </row>
@@ -11729,7 +11705,7 @@
         <v>16</v>
       </c>
       <c r="E340" s="7">
-        <f>C340-B340</f>
+        <f t="shared" si="5"/>
         <v>134531.02142800001</v>
       </c>
     </row>
@@ -11747,7 +11723,7 @@
         <v>16</v>
       </c>
       <c r="E341" s="7">
-        <f>C341-B341</f>
+        <f t="shared" si="5"/>
         <v>98815.407611000002</v>
       </c>
     </row>
@@ -11762,7 +11738,7 @@
         <v>0</v>
       </c>
       <c r="E342" s="7" t="e">
-        <f>C342-B342</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11777,7 +11753,7 @@
         <v>0</v>
       </c>
       <c r="E343" s="7" t="e">
-        <f>C343-B343</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11795,7 +11771,7 @@
         <v>0</v>
       </c>
       <c r="E344" s="7">
-        <f>C344-B344</f>
+        <f t="shared" si="5"/>
         <v>28694</v>
       </c>
     </row>
@@ -11810,7 +11786,7 @@
         <v>0</v>
       </c>
       <c r="E345" s="7" t="e">
-        <f>C345-B345</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11825,7 +11801,7 @@
         <v>0</v>
       </c>
       <c r="E346" s="7" t="e">
-        <f>C346-B346</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11840,7 +11816,7 @@
         <v>16</v>
       </c>
       <c r="E347" s="7" t="e">
-        <f>C347-B347</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11855,7 +11831,7 @@
         <v>16</v>
       </c>
       <c r="E348" s="7" t="e">
-        <f>C348-B348</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11873,7 +11849,7 @@
         <v>0</v>
       </c>
       <c r="E349" s="7">
-        <f>C349-B349</f>
+        <f t="shared" si="5"/>
         <v>3.838028</v>
       </c>
     </row>
@@ -11888,7 +11864,7 @@
         <v>16</v>
       </c>
       <c r="E350" s="7" t="e">
-        <f>C350-B350</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11903,7 +11879,7 @@
         <v>0</v>
       </c>
       <c r="E351" s="7" t="e">
-        <f>C351-B351</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11921,7 +11897,7 @@
         <v>0</v>
       </c>
       <c r="E352" s="7">
-        <f>C352-B352</f>
+        <f t="shared" si="5"/>
         <v>27729565.161343999</v>
       </c>
     </row>
@@ -11936,7 +11912,7 @@
         <v>0</v>
       </c>
       <c r="E353" s="7" t="e">
-        <f>C353-B353</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11954,7 +11930,7 @@
         <v>16</v>
       </c>
       <c r="E354" s="7" t="e">
-        <f>C354-B354</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11969,7 +11945,7 @@
         <v>16</v>
       </c>
       <c r="E355" s="7" t="e">
-        <f>C355-B355</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11984,7 +11960,7 @@
         <v>0</v>
       </c>
       <c r="E356" s="7" t="e">
-        <f>C356-B356</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -11999,7 +11975,7 @@
         <v>0</v>
       </c>
       <c r="E357" s="7" t="e">
-        <f>C357-B357</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -12017,7 +11993,7 @@
         <v>0</v>
       </c>
       <c r="E358" s="7">
-        <f>C358-B358</f>
+        <f t="shared" si="5"/>
         <v>0.33333333333333037</v>
       </c>
     </row>
@@ -12032,7 +12008,7 @@
         <v>0</v>
       </c>
       <c r="E359" s="7" t="e">
-        <f>C359-B359</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -12047,7 +12023,7 @@
         <v>16</v>
       </c>
       <c r="E360" s="7" t="e">
-        <f>C360-B360</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -12062,7 +12038,7 @@
         <v>11</v>
       </c>
       <c r="E361" s="7" t="e">
-        <f>C361-B361</f>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -12080,7 +12056,7 @@
         <v>0</v>
       </c>
       <c r="E362" s="7">
-        <f>C362-B362</f>
+        <f t="shared" si="5"/>
         <v>62535.736428289674</v>
       </c>
     </row>
@@ -12096,7 +12072,7 @@
   </sheetData>
   <autoFilter ref="A1:E362">
     <sortState ref="A2:E362">
-      <sortCondition sortBy="cellColor" ref="E1:E362" dxfId="1"/>
+      <sortCondition sortBy="cellColor" ref="E1:E362" dxfId="0"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>